<commit_message>
made few changes in code.
</commit_message>
<xml_diff>
--- a/bin/testcases/printing.xlsx
+++ b/bin/testcases/printing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>TCID</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>sendbutton</t>
+  </si>
+  <si>
+    <t>navigating to Gmail</t>
+  </si>
+  <si>
+    <t>gmail_account</t>
+  </si>
+  <si>
+    <t>storing text value</t>
+  </si>
+  <si>
+    <t>store</t>
   </si>
 </sst>
 </file>
@@ -436,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +459,7 @@
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -590,7 +602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -610,6 +622,47 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Junit to the Project
</commit_message>
<xml_diff>
--- a/bin/testcases/printing.xlsx
+++ b/bin/testcases/printing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="12840" windowHeight="6570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="3690"/>
   </bookViews>
   <sheets>
     <sheet name="Teststeps" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
made changes in code
</commit_message>
<xml_diff>
--- a/bin/testcases/printing.xlsx
+++ b/bin/testcases/printing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>TCID</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>store</t>
+  </si>
+  <si>
+    <t>verify emailid</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>abc.xyz04071991@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -448,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -559,114 +568,135 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>